<commit_message>
feat(catalogue): refined study and datasource views
</commit_message>
<xml_diff>
--- a/backend/molgenis-emx2-io/src/test/resources/HealthDataCatalogue.xlsx
+++ b/backend/molgenis-emx2-io/src/test/resources/HealthDataCatalogue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/umcg-mswertz/git/molgenis-emx2/backend/molgenis-emx2-io/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B5D2C35-1FA7-1949-BDB7-2BFB6929F00B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7080E8F3-89B4-3C4F-960A-1ACF0D6FA120}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{581C931B-D7B9-8D4C-B6C4-1C49EA2AAD8C}"/>
   </bookViews>
@@ -1236,12 +1236,6 @@
     <t>lessCommonContent</t>
   </si>
   <si>
-    <t>contents</t>
-  </si>
-  <si>
-    <t>Contents</t>
-  </si>
-  <si>
     <t>Contributors to the catalogue such as universities, companies, medical centres and research institutes</t>
   </si>
   <si>
@@ -1258,6 +1252,12 @@
   </si>
   <si>
     <t>Collaborations of multiple institutions, addressing research questions using data sources and/or data banks</t>
+  </si>
+  <si>
+    <t>keywords</t>
+  </si>
+  <si>
+    <t>Keywords</t>
   </si>
 </sst>
 </file>
@@ -1711,8 +1711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6827AF39-8A78-C843-9B70-9944F4620E8F}">
   <dimension ref="A1:L230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A156" workbookViewId="0">
-      <selection activeCell="F162" sqref="F162"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1788,7 +1788,7 @@
         <v>14</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -2757,14 +2757,14 @@
       </c>
       <c r="B43" s="7"/>
       <c r="C43" s="7" t="s">
-        <v>400</v>
+        <v>406</v>
       </c>
       <c r="D43" s="7" t="s">
         <v>32</v>
       </c>
       <c r="E43" s="7"/>
       <c r="F43" s="7" t="s">
-        <v>401</v>
+        <v>407</v>
       </c>
       <c r="G43" s="7"/>
       <c r="H43" s="7"/>
@@ -3196,7 +3196,7 @@
         <v>143</v>
       </c>
       <c r="L59" s="6" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">
@@ -3272,7 +3272,7 @@
         <v>143</v>
       </c>
       <c r="L62" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.2">
@@ -3468,7 +3468,7 @@
       </c>
       <c r="K70" s="6"/>
       <c r="L70" s="6" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.2">
@@ -3564,7 +3564,7 @@
         <v>143</v>
       </c>
       <c r="L74" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.2">
@@ -3636,7 +3636,7 @@
         <v>176</v>
       </c>
       <c r="L77" s="6" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.2">
@@ -5259,14 +5259,14 @@
       </c>
       <c r="B145" s="11"/>
       <c r="C145" s="11" t="s">
-        <v>400</v>
+        <v>406</v>
       </c>
       <c r="D145" s="11" t="s">
         <v>32</v>
       </c>
       <c r="E145" s="11"/>
       <c r="F145" s="11" t="s">
-        <v>401</v>
+        <v>407</v>
       </c>
       <c r="G145" s="11"/>
       <c r="H145" s="11"/>
@@ -5551,14 +5551,14 @@
       </c>
       <c r="B157" s="11"/>
       <c r="C157" s="11" t="s">
-        <v>400</v>
+        <v>406</v>
       </c>
       <c r="D157" s="11" t="s">
         <v>32</v>
       </c>
       <c r="E157" s="11"/>
       <c r="F157" s="11" t="s">
-        <v>401</v>
+        <v>407</v>
       </c>
       <c r="G157" s="11"/>
       <c r="H157" s="11"/>
@@ -5641,14 +5641,14 @@
       </c>
       <c r="B161" s="11"/>
       <c r="C161" s="11" t="s">
-        <v>400</v>
+        <v>406</v>
       </c>
       <c r="D161" s="15" t="s">
         <v>32</v>
       </c>
       <c r="E161" s="11"/>
       <c r="F161" s="11" t="s">
-        <v>401</v>
+        <v>407</v>
       </c>
       <c r="G161" s="11"/>
       <c r="H161" s="11"/>
@@ -6793,7 +6793,7 @@
     </row>
     <row r="209" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A209" s="16" t="s">
-        <v>401</v>
+        <v>407</v>
       </c>
       <c r="B209" s="16" t="s">
         <v>370</v>

</xml_diff>